<commit_message>
Updated households with representants info
</commit_message>
<xml_diff>
--- a/data/processed/poland/D/household_family_structure.xlsx
+++ b/data/processed/poland/D/household_family_structure.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="legend" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="processed" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,45 +21,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="27">
+  <si>
+    <t xml:space="preserve">family_count_in_household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relationship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family_structure_regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bez osób spoza rodziny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A(A|C)C*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z krewnymi w linii prostej starszego pokolenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">członek rodziny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A(A|C)C*E+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">krewny starszego pokolenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EA(A|C)C*E?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">np.małżeństwo z dziećmi i ojciec męża</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inna osoba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A(A|C)C*E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z innymi osobami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA(A|C)C*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">np. małżeństwo i brat żony, dziadkowie z wnuczką</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spokrewnione w linii prostej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">członek rodziny młodszego pokolenia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(A(A|C)C*)(E(E|A)A*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">członek rodziny starszego pokolenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(E(E|A)A*)(A(A|C)C*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niespokrewnione w linii prostej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(A(A|C)C*E?){2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(A(A|C)C*E?){3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A+</t>
+  </si>
   <si>
     <t xml:space="preserve">family_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relationship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">house master</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bez osób spoza rodziny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z krewnymi w linii prostej starszego pokolenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">członek rodziny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">krewny starszego pokolenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inna osoba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z innymi osobami</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spokrewnione w linii prostej</t>
-  </si>
-  <si>
-    <t xml:space="preserve">członek rodziny młodszego pokolenia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">członek rodziny starszego pokolenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niespokrewnione w linii prostej</t>
   </si>
 </sst>
 </file>
@@ -68,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -97,6 +140,20 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,13 +205,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -174,23 +239,228 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="35.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -198,229 +468,250 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="n">
-        <v>1</v>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="H1" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="I1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="J1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="K1" s="1" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>5</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>0.886731127964093</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>0.829293554677329</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>0.737467823687074</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>0.413636842659922</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>0.227197346600332</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>0.140304781923279</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>0.0493337113694358</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>0.0719864837371405</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>0.152571398461376</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>0.0938489371325193</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>0.0391487125591172</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.0342604861621428</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.0316411467593698</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.0454473601011698</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.0272878034072064</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.00801366263794009</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0.0342604861621428</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0.0316411467593698</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0.0454473601011698</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>0.0272878034072064</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0.00801366263794009</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>6.19200523666729E-005</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>6.19200523666729E-005</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0</v>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>0.0647483263223066</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>0.0583994551035392</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>0.0717936558119928</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>0.0627167194331374</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="K6" s="0" t="n">
         <v>0.0514976353126642</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>0.00565896900296836</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>0.00450247237923379</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>0.00379386658235852</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>0.00143223277551636</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="K7" s="0" t="n">
         <v>0.00512348922753547</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0</v>
@@ -429,30 +720,33 @@
         <v>0</v>
       </c>
       <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>0.0188856159718352</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>0.0636789967330594</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>0.142243328810493</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="K8" s="0" t="n">
         <v>0.105491329479769</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0</v>
@@ -461,30 +755,33 @@
         <v>0</v>
       </c>
       <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>0.0678201487850401</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="I9" s="0" t="n">
         <v>0.217330593318579</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="J9" s="0" t="n">
         <v>0.35308306950098</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="K9" s="0" t="n">
         <v>0.328034682080925</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0</v>
@@ -493,27 +790,30 @@
         <v>0</v>
       </c>
       <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>0.00138877831736681</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>0.0105648645800401</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="J10" s="0" t="n">
         <v>0.0149253731343284</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="K10" s="0" t="n">
         <v>0.0151077246452969</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0</v>
@@ -522,24 +822,27 @@
         <v>0</v>
       </c>
       <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
         <v>0.00242372776406691</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="I11" s="0" t="n">
         <v>0.0189429866160818</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="J11" s="0" t="n">
         <v>0.0448515000753807</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="K11" s="0" t="n">
         <v>0.0840777719390436</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>0</v>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0</v>
@@ -554,35 +857,41 @@
         <v>0</v>
       </c>
       <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
         <v>0.0315845017337555</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="K12" s="0" t="n">
         <v>0.22320021019443</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
+      <c r="D13" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0" t="n">
         <v>0.113268872035907</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="G13" s="0" t="n">
         <v>0.0167049524658176</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>0.00542242744296721</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="I13" s="0" t="n">
         <v>0.00223943513541996</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="J13" s="0" t="n">
         <v>0.000829187396351576</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="K13" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>